<commit_message>
Added time & damage for custom weapons
</commit_message>
<xml_diff>
--- a/Damage.xlsx
+++ b/Damage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test PULL\PvP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EC6459-BAB8-43F8-8A9A-2C22D768FAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E185C0-6204-4E97-BF73-A6A9A6996F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD5654F4-3E5C-438C-9AE4-71B49168640E}"/>
   </bookViews>
@@ -917,6 +917,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -925,124 +937,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1455,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A4DA1-4750-40CD-A22F-909E221692F2}">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,37 +1366,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="71" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="71" t="s">
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="73"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="77"/>
       <c r="N1" s="24" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="25"/>
       <c r="P1" s="25"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="73"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="77"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2065,37 +1965,37 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="71" t="s">
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="71" t="s">
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="71" t="s">
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="71" t="s">
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="S10" s="72"/>
-      <c r="T10" s="72"/>
-      <c r="U10" s="73"/>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="77"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -2161,7 +2061,7 @@
       <c r="U11" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="V11" s="74" t="s">
+      <c r="V11" s="71" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3096,7 +2996,7 @@
         <f t="shared" si="24"/>
         <v>15</v>
       </c>
-      <c r="V22" s="75">
+      <c r="V22" s="72">
         <f>8/3</f>
         <v>2.6666666666666665</v>
       </c>
@@ -3182,7 +3082,7 @@
         <f t="shared" si="24"/>
         <v>15</v>
       </c>
-      <c r="V23" s="76">
+      <c r="V23" s="73">
         <f>18/3</f>
         <v>6</v>
       </c>
@@ -3268,7 +3168,7 @@
         <f t="shared" si="24"/>
         <v>12.5</v>
       </c>
-      <c r="V24" s="76">
+      <c r="V24" s="73">
         <f>21/3</f>
         <v>7</v>
       </c>
@@ -3354,7 +3254,7 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-      <c r="V25" s="77">
+      <c r="V25" s="74">
         <f>42/3</f>
         <v>14</v>
       </c>
@@ -3376,21 +3276,21 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="71" t="s">
+      <c r="A28" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="71" t="s">
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="73"/>
-      <c r="H28" s="71" t="s">
+      <c r="G28" s="77"/>
+      <c r="H28" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="73"/>
+      <c r="I28" s="77"/>
     </row>
     <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38" t="s">
@@ -3641,6 +3541,10 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A10:E10"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="J1:M1"/>
@@ -3649,48 +3553,44 @@
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="R10:U10"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:I8 N3:Q8 F12:I25 N12:Q25">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:M8">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:U8">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I35">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:M25">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R12:U25">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:F35 H30:H35">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G35">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3719,10 +3619,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="73"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="42" t="s">
@@ -3744,16 +3644,16 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H4" s="71" t="s">
+      <c r="H4" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="71" t="s">
+      <c r="I4" s="76"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="73"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="77"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="45" t="s">
@@ -3926,19 +3826,19 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="71" t="s">
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="73"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="77"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">

</xml_diff>